<commit_message>
Updating Cap 3, 8 and 9
</commit_message>
<xml_diff>
--- a/1) Requirements/3. SWRA_20190405.xlsx
+++ b/1) Requirements/3. SWRA_20190405.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC01B660-CD6B-44C4-B573-221F39F2DAD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,53 +19,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>REQUISITOS DE SOFTWARE</t>
   </si>
   <si>
-    <t>SE DEBE CONTROLAR LA VELOCIDAD DE UN MOTOR DE CORRIENTE DIRECTA MEDIANTE UNA SEÑAL CUADRADA QUE VARIA EN SU ANCHO DE PULSO</t>
-  </si>
-  <si>
-    <t>LA FRECUENCIA DE TRABAJO DE LA SEÑAL CUADRADA DEBE SER CONSTANTE, ENTRE UN RANGO DE 100 Hz A 1000 Hz</t>
-  </si>
-  <si>
     <t>SE DEBE MEDIR LA VELOCIDAD DEL MOTOR MEDIANTE EL USO DE UN SENSOR DE EFECTO HALL ACOPLADO AL MOTOR, EL CUAL DA 4 PULSOS POR CADA VUELTA DEL MOTOR</t>
   </si>
   <si>
     <t>EL VOLTAJE DE ALIMENTACION DE LA TARJETA DE POTENCIA DEBE SER DE 12 V</t>
   </si>
   <si>
-    <t xml:space="preserve">EL MOTOR DEBE SEGUIR EL VALOR DE REFERENCIA </t>
-  </si>
-  <si>
     <t>LA PANTALLA LCD DEBE MOSTRAR LA VELOCIDAD DEL MOTOR Y SETPOINT, AL IGUAL QUE EL PORCENTAJE DE TRABAJO DE LA SEÑAL CUADRADA</t>
   </si>
   <si>
     <t>PARA MEDIR LA VELOCIDAD SE DEBE CONSIDERAR EL NUMERO DE PULSOS REGISTRADOS POR EL SENSOR DE EFECTO HALL, OCURRIDOS EN 100 ms Y PROMEDIARSE CON LOS SIGUIENTES 100 ms</t>
   </si>
   <si>
-    <t>EL VALOR DE REFERENCIA DADO POR EL POTENCIOMETRO SE DIVIDIRA EN 0 V = 0 RPM, 1.5 V = 1500 RPM, 3 V = 3000 RPM, 3.3 V = 3000 RPM</t>
-  </si>
-  <si>
-    <t>SE DEBE PROMEDIAR EL VALOR DE REFERENCIA EN 100 ms, CONSIDERANDO 3 MUESTRAS</t>
-  </si>
-  <si>
     <t>LA PANTALLA LCD DEBE MOSTRAR LOS VALORES ANTERIORMENTE INDICADOS, CON EL FORMATO MOSTRADO EN EL DOCUMENTO DE REQUISITOS DEL SISTEMA, PAGINA 8</t>
   </si>
   <si>
-    <t>EL ALGORITMO DE CONTROL DEBE SER DE LAZO CERRADO</t>
-  </si>
-  <si>
     <t>EL TIEMPO DEFINIDO PARA LA ACCION DE CONTROL DEBE SER DE 100 ms</t>
   </si>
   <si>
-    <t>EL SISTEMA DEBE CONTAR CON UN SISTEMA QUE CONTROLE LOS TIEMPOS DE EJECUCION DEL CODIGO, ABIERTO A LAS OPCIONES QUE SE MUESTRAN EN EL DOCUMENTO DE REQUISITOS DEL SISTEMA, PAGINA 9</t>
-  </si>
-  <si>
     <t>DURANTE LA INICIALIZACION SE DEBE CONSIDERAR LA CONFIGURACION DE LOS REGISTROS MOSTRADOS EN EL DOCUMENTO DE REQUISITOS DEL SISTEMA, PAGINA 9</t>
   </si>
   <si>
@@ -92,13 +67,108 @@
   </si>
   <si>
     <t>SE DEBE CONSIDERAR QUE EL DISEÑO DE CODIGO SEA MODULAR, REUTILIZABLE, MANTENIBLE, BASADO EN PRUEBAS</t>
+  </si>
+  <si>
+    <t>TIPO DE REQUISITO</t>
+  </si>
+  <si>
+    <t>SE DEBE CONTROLAR LA VELOCIDAD DE UN MOTOR DE CORRIENTE DIRECTA MEDIANTE UNA SEÑAL CUADRADA QUE VARIA EN SU ANCHO DE PULSO Y CUYA FRECUENCIA DE TRABAJO DEBE SER CONSTANTE.</t>
+  </si>
+  <si>
+    <t>2. LA FRECUENCIA DE TRABAJO DE LA SEÑAL CUADRADA DEBE DE SER DE 1 KHZ.</t>
+  </si>
+  <si>
+    <t>EL MOTOR DEBE SEGUIR EL VALOR DE REFERENCIA O “SETPOINT” (VELOCIDAD DESEADA), EL CUAL ESTARÁ DADO POR EL AJUSTE DE UNA RESISTENCIA VARIABLE (POTENCIÓMETRO).</t>
+  </si>
+  <si>
+    <t>AJUSTE DEL VALOR DE REFERENCIA O SETPOINT MEDIANTE POTENCIÓMETRO DEBE DE DAR UNA SALIDA DE 0 A 3000 RPM.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">EL CIRCUITO DEL MOTOR </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DEBE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PROPORCIONAR UNA SALIDA ESTANDARIZADA DE 3.3V TANTO DEL SENSOR DE EFECTO HALL COMO DE LA SEÑAL DE NFAULT.</t>
+    </r>
+  </si>
+  <si>
+    <t>EL DRIVER DEL MOTOR USARÁ EL DRV8848-2A CONFIGURADO COMO MEDIO PUENTE H.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LA VELOCIDAD DEL MOTOR SERA DIRECTAMENTE  PROPORCIONAL AL CICLO DE TRABAJO DE LA SEÑAL CUADRADA.</t>
+    </r>
+  </si>
+  <si>
+    <t>EL ALGORITMO DE CONTROL DEBE SER EN LAZO CERRADO Y SERÁ DEL TIPO: PROPORCIONAL + INTEGRAL</t>
+  </si>
+  <si>
+    <t>EL SISTEMA DEBE CONTAR CON UN SISTEMA DE CONTROL DE TIEMPO PARA HACER DETERMINÍSTICOS LOS PROCESOS DEL CÓDIGO, POR LO QUE SE USARA EL SISTEMA OPERATIVO DE RENESAS  XTHREAD QUE SE BASA EN TAREAS PREENTRANTES.</t>
+  </si>
+  <si>
+    <t>PARA ATENUAR EL RUIDO QUE PUEDA HABER EN LA RESISTENCIA, SE DEBE PROMEDIAR EL VALOR DE REFERENCIA CON UN PERIODO DE 100 ms, CONSIDERANDO 3 MUESTRAS</t>
+  </si>
+  <si>
+    <t>LOS DIAGNÓSTICOS DE CORTOS Y LOS CONTROLES DIGITALES DEBEN SER GUARDADOS EN LA MEMORIA EEPROM.</t>
+  </si>
+  <si>
+    <t>EL SISTEMA DEBE DETECTAR UN CORTO A BATERÍA.</t>
+  </si>
+  <si>
+    <t>EL SISTEMA DEBE DETECTAR UN CORTO A TIERRA.</t>
+  </si>
+  <si>
+    <t>SYSTEM</t>
+  </si>
+  <si>
+    <t>EL SISTEMA DEBE SER MONITOREADO POR UN WATCHDOG TIMER</t>
+  </si>
+  <si>
+    <t>SOFTWARE</t>
+  </si>
+  <si>
+    <t>REQ. NO.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,16 +184,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,14 +241,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,205 +564,354 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="155.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D15" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="D17" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="5">
+        <v>16</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D19" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="5">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D21" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>20</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>21</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
+        <v>22</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>23</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D25" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <v>24</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D26" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <v>25</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D27" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>26</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D28" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="5">
+        <v>27</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D29" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="5">
+        <v>28</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D30" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="5">
+        <v>29</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
+      <c r="D31" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualizo Cap 11
</commit_message>
<xml_diff>
--- a/1) Requirements/3. SWRA_20190405.xlsx
+++ b/1) Requirements/3. SWRA_20190405.xlsx
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>SE DEBE CONTROLAR LA VELOCIDAD DE UN MOTOR DE CORRIENTE DIRECTA MEDIANTE UNA SEÑAL CUADRADA QUE VARIA EN SU ANCHO DE PULSO Y CUYA FRECUENCIA DE TRABAJO DEBE SER CONSTANTE.</t>
-  </si>
-  <si>
-    <t>2. LA FRECUENCIA DE TRABAJO DE LA SEÑAL CUADRADA DEBE DE SER DE 1 KHZ.</t>
   </si>
   <si>
     <t>EL MOTOR DEBE SEGUIR EL VALOR DE REFERENCIA O “SETPOINT” (VELOCIDAD DESEADA), EL CUAL ESTARÁ DADO POR EL AJUSTE DE UNA RESISTENCIA VARIABLE (POTENCIÓMETRO).</t>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>REQ. NO.</t>
+  </si>
+  <si>
+    <t>LA FRECUENCIA DE TRABAJO DE LA SEÑAL CUADRADA DEBE DE SER DE 1 KHZ.</t>
   </si>
 </sst>
 </file>
@@ -567,9 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -585,7 +583,7 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
@@ -602,7 +600,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -610,10 +608,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -624,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -635,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -643,10 +641,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -658,7 +656,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -669,7 +667,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -677,10 +675,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -688,10 +686,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -699,10 +697,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
@@ -710,10 +708,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -721,10 +719,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
@@ -735,7 +733,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
@@ -743,10 +741,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -757,7 +755,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
@@ -765,10 +763,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -779,7 +777,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -787,10 +785,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -801,7 +799,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -809,10 +807,10 @@
         <v>20</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -820,10 +818,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -831,10 +829,10 @@
         <v>22</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -845,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -856,7 +854,7 @@
         <v>10</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -867,7 +865,7 @@
         <v>11</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -878,7 +876,7 @@
         <v>12</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -889,7 +887,7 @@
         <v>13</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -900,7 +898,7 @@
         <v>14</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -911,7 +909,7 @@
         <v>15</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>